<commit_message>
updated excel to remove names
</commit_message>
<xml_diff>
--- a/assets/SIT User Study.xlsx
+++ b/assets/SIT User Study.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\chat_bot\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\SIT_Chatbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49646E4A-F0A5-46B6-93EA-B626372280B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640BE7AB-7C4F-4001-9737-36672AFBD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="91">
   <si>
     <t>Chatbot (time)</t>
   </si>
@@ -172,9 +172,6 @@
     <t>An email that I can reach out to, to find out more about the admission process</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Have they visited SIT's website before?</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Joey</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -205,181 +199,115 @@
     <t>Its me</t>
   </si>
   <si>
-    <t>Josh</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>User was actually using search bar to search for the queries rather than navigating through the different tabs</t>
   </si>
   <si>
-    <t>Yong Chun</t>
-  </si>
-  <si>
     <t>even faster</t>
   </si>
   <si>
-    <t>Elsha</t>
-  </si>
-  <si>
     <t>suprisingly specific, dont need to ask many questions but not enough personality</t>
   </si>
   <si>
-    <t>Jerald</t>
-  </si>
-  <si>
     <t>abit slow but is like googling but easier because it understands the context</t>
   </si>
   <si>
     <t>uses search bar sometimes but gets distracted very easily</t>
   </si>
   <si>
-    <t>Aziza Kanimetova</t>
-  </si>
-  <si>
     <t>the chatbot is quicker, the website not all the pages are well deisgn, For example for the deadline you have to go to the QnA part to find out</t>
   </si>
   <si>
     <t>it is unable to recognise the difference between the word "course fee" and "cost"</t>
   </si>
   <si>
-    <t>Patrick Lim</t>
-  </si>
-  <si>
     <t>all the question can be link to a single subject</t>
   </si>
   <si>
     <t>Uses search bar too to search for answers rather than navigating within the website</t>
   </si>
   <si>
-    <t>Cristina Ng</t>
-  </si>
-  <si>
     <t>faster, its better than the search engine, tell the school that my mother says so, most places have a small chabot currently now at the side of the portal to assist with searches</t>
   </si>
   <si>
     <t>users search bar too to search for answers</t>
   </si>
   <si>
-    <t>Lester</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
     <t>Doubting the reliability of the language model, afraid of not getting accurate data and I will visit the website anyway to confirm if the data real</t>
   </si>
   <si>
-    <t>Jack Ong</t>
-  </si>
-  <si>
     <t>It is faster and allows me to ask the question that I need instead of going to the link and trial and error</t>
   </si>
   <si>
     <t xml:space="preserve">Chatbot crashed </t>
   </si>
   <si>
-    <t>Matthew Wong</t>
-  </si>
-  <si>
     <t>Because some of the website information is so stupid and hard to find</t>
   </si>
   <si>
     <t>It got the question about the undergraduate application deadline wrong because of its inability to understand the users question</t>
   </si>
   <si>
-    <t>Chen Lei</t>
-  </si>
-  <si>
     <t>I do not need to find where the material is, just asking can get what I want</t>
   </si>
   <si>
-    <t>Wen Jun</t>
-  </si>
-  <si>
     <t>I can just ask it questions and immediately get the answer</t>
   </si>
   <si>
     <t>User uses search bar at times to search for answers in the SIT website</t>
   </si>
   <si>
-    <t>Hong Wei</t>
-  </si>
-  <si>
     <t>The wbesite is very confusing in general and the way that is it categorise can be quite confusing for example whem looking for an email about admission, why isit not under the admission tab but rather in the contact us page</t>
   </si>
   <si>
     <t>EDE was not recognise properly and it led to the general course page</t>
   </si>
   <si>
-    <t>Justin</t>
-  </si>
-  <si>
     <t>Faster and I dont have to look through so much bullshit and I can just type key words easy</t>
   </si>
   <si>
     <t>it didnt recognise application but could only recogise admission for the last question</t>
   </si>
   <si>
-    <t>Samantha Lim</t>
-  </si>
-  <si>
     <t>It is so much more convienent, you just need to type in key words and you dont have to squnich your eyes to look for everything on the website</t>
   </si>
   <si>
     <t>Uses the search function to search sometiems</t>
   </si>
   <si>
-    <t>Jeremy Wong</t>
-  </si>
-  <si>
     <t>It just goes direct to the point, you dont need to go through pages where you think that the information is there but it is not</t>
   </si>
   <si>
     <t>Does not recongise EDE again but manage to still provide the correct course link</t>
   </si>
   <si>
-    <t>Jamie</t>
-  </si>
-  <si>
     <t>Because I like to see the vibrant colors and the human touch in it. The visuals make it more appealing than the chatbot</t>
   </si>
   <si>
     <t>Use search bar in sit website to search for info but cannot find someimtes.</t>
   </si>
   <si>
-    <t>Meg</t>
-  </si>
-  <si>
     <t>I think it allows me to just use natural language to ask my questions instead of clicking around to find what I am looking for when i dont know where anything is</t>
   </si>
   <si>
     <t>Did not get the correct answer for application deadline</t>
   </si>
   <si>
-    <t>Tania</t>
-  </si>
-  <si>
     <t>I think that the website will provide me to have more information that I would think initially that I wouldnt need, because I would have stuff that I would have overlook if I were to use the chatbot</t>
   </si>
   <si>
-    <t>Triston</t>
-  </si>
-  <si>
     <t>if I am looking casually, fast and straight foward information then it is chatbot, but if I require more indepth I will use the website</t>
   </si>
   <si>
-    <t>Angela</t>
-  </si>
-  <si>
     <t>I can see all the information and it is more reliable</t>
   </si>
   <si>
     <t>unable to understand immediately question 5, chinese is direct translated surprisingly when asked a chinese question</t>
-  </si>
-  <si>
-    <t>Xin Bei</t>
   </si>
   <si>
     <t>I mean chatbot is the lazier option, you dont have to navigate through the ui, the user thought that the chatbot was dead because there was no loading bar</t>
@@ -2703,7 +2631,7 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
@@ -3211,24 +3139,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="80.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
@@ -3244,549 +3171,477 @@
       <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
sucessfully change vizz folder
</commit_message>
<xml_diff>
--- a/assets/SIT User Study.xlsx
+++ b/assets/SIT User Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\SIT_Chatbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5E8297-386E-4CB9-8D4C-A9C338BAEA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAFEC70-97B1-45FA-87D5-2CC56C2EA34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
@@ -1243,9 +1243,9 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
pushing updates again on update of excel sheet
</commit_message>
<xml_diff>
--- a/assets/SIT User Study.xlsx
+++ b/assets/SIT User Study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\SIT_Chatbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4229015D-69AE-479D-8625-1178C7743400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C58DB1-BC17-4AA3-9C59-F5BD7A825239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="87">
   <si>
     <t>Chatbot (time)</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>SIT Students?</t>
+  </si>
+  <si>
+    <t>nil</t>
   </si>
 </sst>
 </file>
@@ -3781,11 +3784,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3794,11 +3797,11 @@
     <col min="3" max="3" width="30.140625" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="79.42578125" customWidth="1"/>
     <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>85</v>
       </c>
@@ -3817,8 +3820,9 @@
       <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3841,7 +3845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3864,7 +3868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3883,8 +3887,11 @@
       <c r="F4" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3903,8 +3910,11 @@
       <c r="F5" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -3950,7 +3960,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3973,7 +3983,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3996,7 +4006,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -4015,8 +4025,11 @@
       <c r="F10" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -4039,7 +4052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -4062,7 +4075,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4081,8 +4094,11 @@
       <c r="F13" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -4105,7 +4121,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4128,7 +4144,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -4220,7 +4236,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4262,6 +4278,9 @@
       <c r="F21" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -4282,6 +4301,9 @@
       <c r="F22" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -4324,6 +4346,9 @@
       </c>
       <c r="F24" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added more viz and edited data
</commit_message>
<xml_diff>
--- a/assets/SIT User Study.xlsx
+++ b/assets/SIT User Study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\krispy_noodles\SIT_Chatbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC05EAEE-589F-468A-8622-3A6E22BFE2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E3B69D-8B26-4A9A-B040-79BBAD6928EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="99">
   <si>
     <t>Chatbot (time)</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Chatbot</t>
   </si>
   <si>
-    <t>faster</t>
-  </si>
-  <si>
     <t>Its me</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>User was actually using search bar to search for the queries rather than navigating through the different tabs</t>
   </si>
   <si>
-    <t>even faster</t>
-  </si>
-  <si>
     <t>suprisingly specific, dont need to ask many questions but not enough personality</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
     <t>It is faster and allows me to ask the question that I need instead of going to the link and trial and error</t>
   </si>
   <si>
-    <t xml:space="preserve">Chatbot crashed </t>
-  </si>
-  <si>
     <t>Because some of the website information is so stupid and hard to find</t>
   </si>
   <si>
@@ -295,20 +286,62 @@
     <t>SIT Students?</t>
   </si>
   <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>fast</t>
-  </si>
-  <si>
     <t>The wbesite is very confusing in general and the way that is it categorise can be quite confusing for example when looking for an email about admission, why isit not under the admission tab but rather in the contact us page</t>
+  </si>
+  <si>
+    <t>I really prefer the chatbot as it I get my question answered alot faster than the website</t>
+  </si>
+  <si>
+    <t>the chatbot is faster</t>
+  </si>
+  <si>
+    <t>the information retrieval is done alot faster than the website</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Speed &amp; Convenience</t>
+  </si>
+  <si>
+    <t>Effortless Information Access</t>
+  </si>
+  <si>
+    <t>Ability to Understand Context</t>
+  </si>
+  <si>
+    <t>Chatbot crashed</t>
+  </si>
+  <si>
+    <t>Frustration with Website Navigation</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -329,16 +362,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA64D79"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -346,14 +416,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +709,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1247,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,10 +1997,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2533,10 +2639,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3175,10 +3281,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3789,24 +3895,24 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="79.42578125" customWidth="1"/>
-    <col min="7" max="7" width="80.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="80.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>84</v>
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>36</v>
@@ -3821,11 +3927,13 @@
         <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3838,45 +3946,51 @@
       <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
@@ -3884,17 +3998,17 @@
       <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3910,14 +4024,14 @@
       <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3925,7 +4039,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
@@ -3933,22 +4047,25 @@
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>41</v>
@@ -3956,22 +4073,25 @@
       <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>41</v>
@@ -3979,22 +4099,25 @@
       <c r="E8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>41</v>
@@ -4002,37 +4125,38 @@
       <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -4040,7 +4164,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>41</v>
@@ -4048,22 +4172,25 @@
       <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>41</v>
@@ -4071,14 +4198,17 @@
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4086,7 +4216,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
@@ -4094,14 +4224,14 @@
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -4117,45 +4247,51 @@
       <c r="E14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>41</v>
@@ -4163,22 +4299,25 @@
       <c r="E16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>41</v>
@@ -4186,22 +4325,25 @@
       <c r="E17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>41</v>
@@ -4209,14 +4351,17 @@
       <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -4224,22 +4369,23 @@
         <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4255,14 +4401,17 @@
       <c r="E20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -4276,16 +4425,14 @@
         <v>41</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -4301,14 +4448,14 @@
       <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -4322,16 +4469,17 @@
         <v>41</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -4347,40 +4495,47 @@
       <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="F24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>